<commit_message>
segund version del modelo
</commit_message>
<xml_diff>
--- a/divisiones.xlsx
+++ b/divisiones.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
-  <si>
-    <t>audio1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>UPN</t>
   </si>
@@ -38,21 +35,12 @@
     <t>audio3</t>
   </si>
   <si>
-    <t>audio4</t>
-  </si>
-  <si>
-    <t>audio5</t>
-  </si>
-  <si>
     <t>audio6</t>
   </si>
   <si>
     <t>audio7</t>
   </si>
   <si>
-    <t>audio9</t>
-  </si>
-  <si>
     <t>audio10</t>
   </si>
   <si>
@@ -62,12 +50,6 @@
     <t>audio12</t>
   </si>
   <si>
-    <t>audio13</t>
-  </si>
-  <si>
-    <t>audio14</t>
-  </si>
-  <si>
     <t>audio15</t>
   </si>
   <si>
@@ -77,24 +59,12 @@
     <t>audio17</t>
   </si>
   <si>
-    <t>audio18</t>
-  </si>
-  <si>
     <t>audio19</t>
   </si>
   <si>
-    <t>audio20</t>
-  </si>
-  <si>
     <t>audio21</t>
   </si>
   <si>
-    <t>audio22</t>
-  </si>
-  <si>
-    <t>audio23</t>
-  </si>
-  <si>
     <t>audio24</t>
   </si>
   <si>
@@ -110,18 +80,6 @@
     <t>audio28</t>
   </si>
   <si>
-    <t>audio29</t>
-  </si>
-  <si>
-    <t>audio30</t>
-  </si>
-  <si>
-    <t>audio31</t>
-  </si>
-  <si>
-    <t>audio32</t>
-  </si>
-  <si>
     <t>audio33</t>
   </si>
   <si>
@@ -137,15 +95,6 @@
     <t>audio37</t>
   </si>
   <si>
-    <t>audio38</t>
-  </si>
-  <si>
-    <t>audio39</t>
-  </si>
-  <si>
-    <t>MODA</t>
-  </si>
-  <si>
     <t>MOVISTAR</t>
   </si>
   <si>
@@ -155,50 +104,156 @@
     <t>ORO</t>
   </si>
   <si>
+    <t>CERTUS</t>
+  </si>
+  <si>
+    <t>BITEL</t>
+  </si>
+  <si>
+    <t>NOMARCA</t>
+  </si>
+  <si>
+    <t>audio41</t>
+  </si>
+  <si>
+    <t>audio42</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>audio8</t>
+  </si>
+  <si>
+    <t>audio43</t>
+  </si>
+  <si>
+    <t>audio44</t>
+  </si>
+  <si>
+    <t>audio45</t>
+  </si>
+  <si>
+    <t>audio46</t>
+  </si>
+  <si>
+    <t>audio47</t>
+  </si>
+  <si>
+    <t>audio48</t>
+  </si>
+  <si>
+    <t>audio50</t>
+  </si>
+  <si>
+    <t>audio51</t>
+  </si>
+  <si>
+    <t>audio52</t>
+  </si>
+  <si>
+    <t>audio53</t>
+  </si>
+  <si>
+    <t>audio54</t>
+  </si>
+  <si>
+    <t>audio55</t>
+  </si>
+  <si>
+    <t>audio56</t>
+  </si>
+  <si>
+    <t>audio57</t>
+  </si>
+  <si>
+    <t>audio58</t>
+  </si>
+  <si>
+    <t>audio59</t>
+  </si>
+  <si>
+    <t>audio60</t>
+  </si>
+  <si>
+    <t>audio61</t>
+  </si>
+  <si>
+    <t>audio62</t>
+  </si>
+  <si>
+    <t>audio63</t>
+  </si>
+  <si>
+    <t>audio67</t>
+  </si>
+  <si>
+    <t>audio69</t>
+  </si>
+  <si>
+    <t>audio72</t>
+  </si>
+  <si>
+    <t>audio76</t>
+  </si>
+  <si>
+    <t>audio77</t>
+  </si>
+  <si>
+    <t>audio78</t>
+  </si>
+  <si>
+    <t>audio79</t>
+  </si>
+  <si>
+    <t>audio80</t>
+  </si>
+  <si>
+    <t>audio81</t>
+  </si>
+  <si>
+    <t>audio82</t>
+  </si>
+  <si>
+    <t>audio88</t>
+  </si>
+  <si>
+    <t>audio89</t>
+  </si>
+  <si>
+    <t>DIRECTV</t>
+  </si>
+  <si>
+    <t>KART</t>
+  </si>
+  <si>
+    <t>NESQUIK</t>
+  </si>
+  <si>
+    <t>ONCOSALUD</t>
+  </si>
+  <si>
+    <t>PERUCHAMPS</t>
+  </si>
+  <si>
+    <t>UBER</t>
+  </si>
+  <si>
     <t>CINEMARK</t>
-  </si>
-  <si>
-    <t>CERTUS</t>
-  </si>
-  <si>
-    <t>BITEL</t>
-  </si>
-  <si>
-    <t>NOMARCA</t>
-  </si>
-  <si>
-    <t>audio40</t>
-  </si>
-  <si>
-    <t>audio41</t>
-  </si>
-  <si>
-    <t>audio42</t>
-  </si>
-  <si>
-    <t>audio</t>
-  </si>
-  <si>
-    <t>folder</t>
-  </si>
-  <si>
-    <t>cantidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -226,9 +281,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,34 +563,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,10 +601,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,10 +612,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -566,73 +623,73 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9">
         <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -640,153 +697,153 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -794,189 +851,365 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C32">
-        <v>7</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C33">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C36">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C37">
-        <v>70</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C38">
-        <v>45</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C39">
-        <v>45</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C40">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C41">
-        <v>60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C42">
-        <v>20</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>